<commit_message>
pipeline running with larger dataset
</commit_message>
<xml_diff>
--- a/app/Data/raw_data/manual_game_tagging.xlsx
+++ b/app/Data/raw_data/manual_game_tagging.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seelc\OneDrive\Desktop\Lucas Desktop Items\Projects\optigame_simple\optigame_simple\app\Data\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51D7C07-3781-4F0B-8E5C-005AC0C60108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDDCF1D-13BF-460B-8AC3-D8C6BE588E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{237F2DA4-652B-41E0-AEDA-F9274CD289A5}"/>
   </bookViews>
@@ -17,6 +17,9 @@
     <sheet name="tags" sheetId="2" r:id="rId2"/>
     <sheet name="tagged_games" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">tagged_games!$A$1:$L$681</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9500" uniqueCount="3534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9657" uniqueCount="3535">
   <si>
     <t>id</t>
   </si>
@@ -10887,6 +10890,9 @@
   </si>
   <si>
     <t>card</t>
+  </si>
+  <si>
+    <t>strategy</t>
   </si>
 </sst>
 </file>
@@ -39821,8 +39827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80090C68-1AA8-4D07-8B4A-954A981011F1}">
   <dimension ref="A1:A59"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40131,18 +40137,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84173DE9-3815-4818-B963-E90EED192D50}">
   <dimension ref="A1:L681"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A662" workbookViewId="0">
+      <selection activeCell="J629" sqref="J629"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="60.5703125" customWidth="1"/>
-    <col min="4" max="6" width="12.5703125" customWidth="1"/>
+    <col min="4" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
     <col min="7" max="8" width="12.5703125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="97.5703125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="14" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -40609,7 +40616,7 @@
         <v>3516</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>595</v>
       </c>
@@ -40637,8 +40644,17 @@
       <c r="I17" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>3487</v>
+      </c>
+      <c r="K17" t="s">
+        <v>3486</v>
+      </c>
+      <c r="L17" t="s">
+        <v>3516</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2098</v>
       </c>
@@ -40666,8 +40682,17 @@
       <c r="I18" t="s">
         <v>2102</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>3503</v>
+      </c>
+      <c r="K18" t="s">
+        <v>3486</v>
+      </c>
+      <c r="L18" t="s">
+        <v>3516</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3085</v>
       </c>
@@ -40696,7 +40721,7 @@
         <v>3089</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1351</v>
       </c>
@@ -40722,7 +40747,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2690</v>
       </c>
@@ -40750,8 +40775,17 @@
       <c r="I21" t="s">
         <v>2694</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>3487</v>
+      </c>
+      <c r="K21" t="s">
+        <v>3517</v>
+      </c>
+      <c r="L21" t="s">
+        <v>3499</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3115</v>
       </c>
@@ -40777,7 +40811,7 @@
         <v>3118</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1169</v>
       </c>
@@ -40806,7 +40840,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1110</v>
       </c>
@@ -40835,7 +40869,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>384</v>
       </c>
@@ -40864,7 +40898,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>2171</v>
       </c>
@@ -40893,7 +40927,7 @@
         <v>2175</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2252</v>
       </c>
@@ -40922,7 +40956,7 @@
         <v>2256</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2311</v>
       </c>
@@ -40951,7 +40985,7 @@
         <v>2315</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>2640</v>
       </c>
@@ -40980,7 +41014,7 @@
         <v>2644</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1793</v>
       </c>
@@ -41009,7 +41043,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>3318</v>
       </c>
@@ -41037,8 +41071,17 @@
       <c r="I31" t="s">
         <v>3322</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>3517</v>
+      </c>
+      <c r="K31" t="s">
+        <v>3505</v>
+      </c>
+      <c r="L31" t="s">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3313</v>
       </c>
@@ -41065,6 +41108,15 @@
       </c>
       <c r="I32" t="s">
         <v>3317</v>
+      </c>
+      <c r="J32" t="s">
+        <v>3517</v>
+      </c>
+      <c r="K32" t="s">
+        <v>3505</v>
+      </c>
+      <c r="L32" t="s">
+        <v>3486</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -41516,7 +41568,7 @@
         <v>3285</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>2275</v>
       </c>
@@ -41542,7 +41594,7 @@
         <v>2278</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>2888</v>
       </c>
@@ -41571,7 +41623,7 @@
         <v>2892</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>1996</v>
       </c>
@@ -41597,7 +41649,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>264</v>
       </c>
@@ -41626,7 +41678,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>250</v>
       </c>
@@ -41652,7 +41704,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>548</v>
       </c>
@@ -41678,7 +41730,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>322</v>
       </c>
@@ -41704,7 +41756,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1671</v>
       </c>
@@ -41730,7 +41782,7 @@
         <v>1674</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>571</v>
       </c>
@@ -41756,7 +41808,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>9</v>
       </c>
@@ -41782,7 +41834,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>3224</v>
       </c>
@@ -41811,7 +41863,7 @@
         <v>3228</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>198</v>
       </c>
@@ -41840,7 +41892,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>1378</v>
       </c>
@@ -41869,7 +41921,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>1980</v>
       </c>
@@ -41897,8 +41949,17 @@
       <c r="I62" t="s">
         <v>1984</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J62" t="s">
+        <v>3532</v>
+      </c>
+      <c r="K62" t="s">
+        <v>3523</v>
+      </c>
+      <c r="L62" t="s">
+        <v>3516</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>1193</v>
       </c>
@@ -41927,7 +41988,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>2949</v>
       </c>
@@ -42408,7 +42469,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>3076</v>
       </c>
@@ -42434,7 +42495,7 @@
         <v>3079</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>2609</v>
       </c>
@@ -42460,7 +42521,7 @@
         <v>2612</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>1648</v>
       </c>
@@ -42489,7 +42550,7 @@
         <v>1652</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>1855</v>
       </c>
@@ -42518,7 +42579,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>1248</v>
       </c>
@@ -42547,7 +42608,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>446</v>
       </c>
@@ -42575,8 +42636,17 @@
       <c r="I86" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J86" t="s">
+        <v>3523</v>
+      </c>
+      <c r="K86" t="s">
+        <v>3522</v>
+      </c>
+      <c r="L86" t="s">
+        <v>3516</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>543</v>
       </c>
@@ -42604,8 +42674,17 @@
       <c r="I87" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J87" t="s">
+        <v>3523</v>
+      </c>
+      <c r="K87" t="s">
+        <v>3522</v>
+      </c>
+      <c r="L87" t="s">
+        <v>3516</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>1101</v>
       </c>
@@ -42631,7 +42710,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>861</v>
       </c>
@@ -42659,8 +42738,17 @@
       <c r="I89" t="s">
         <v>865</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J89" t="s">
+        <v>3487</v>
+      </c>
+      <c r="K89" t="s">
+        <v>3514</v>
+      </c>
+      <c r="L89" t="s">
+        <v>3494</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>1174</v>
       </c>
@@ -42686,7 +42774,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>1512</v>
       </c>
@@ -42715,7 +42803,7 @@
         <v>1516</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>2868</v>
       </c>
@@ -42744,7 +42832,7 @@
         <v>2872</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>769</v>
       </c>
@@ -42773,7 +42861,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>1798</v>
       </c>
@@ -42802,7 +42890,7 @@
         <v>1802</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>2357</v>
       </c>
@@ -42831,7 +42919,7 @@
         <v>2361</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>2357</v>
       </c>
@@ -43818,7 +43906,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>3383</v>
       </c>
@@ -43847,7 +43935,7 @@
         <v>3387</v>
       </c>
     </row>
-    <row r="130" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>400</v>
       </c>
@@ -43876,7 +43964,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>562</v>
       </c>
@@ -43905,7 +43993,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>2504</v>
       </c>
@@ -43933,8 +44021,17 @@
       <c r="I132" t="s">
         <v>2508</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J132" t="s">
+        <v>3486</v>
+      </c>
+      <c r="K132" t="s">
+        <v>3508</v>
+      </c>
+      <c r="L132" t="s">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>2939</v>
       </c>
@@ -43963,7 +44060,7 @@
         <v>2943</v>
       </c>
     </row>
-    <row r="134" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>3033</v>
       </c>
@@ -43992,7 +44089,7 @@
         <v>3037</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>110</v>
       </c>
@@ -44018,7 +44115,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>1077</v>
       </c>
@@ -44044,7 +44141,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>2806</v>
       </c>
@@ -44073,7 +44170,7 @@
         <v>2810</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>667</v>
       </c>
@@ -44102,7 +44199,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>734</v>
       </c>
@@ -44131,7 +44228,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>1747</v>
       </c>
@@ -44159,8 +44256,17 @@
       <c r="I140" t="s">
         <v>1750</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J140" t="s">
+        <v>3486</v>
+      </c>
+      <c r="K140" t="s">
+        <v>3487</v>
+      </c>
+      <c r="L140" t="s">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>974</v>
       </c>
@@ -44189,7 +44295,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>2726</v>
       </c>
@@ -44218,7 +44324,7 @@
         <v>2730</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>3014</v>
       </c>
@@ -44247,7 +44353,7 @@
         <v>3017</v>
       </c>
     </row>
-    <row r="144" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>2993</v>
       </c>
@@ -45180,7 +45286,7 @@
         <v>2753</v>
       </c>
     </row>
-    <row r="177" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>2604</v>
       </c>
@@ -45209,7 +45315,7 @@
         <v>2608</v>
       </c>
     </row>
-    <row r="178" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>2443</v>
       </c>
@@ -45237,8 +45343,17 @@
       <c r="I178" t="s">
         <v>2447</v>
       </c>
-    </row>
-    <row r="179" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J178" t="s">
+        <v>3517</v>
+      </c>
+      <c r="K178" t="s">
+        <v>3508</v>
+      </c>
+      <c r="L178" t="s">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>2651</v>
       </c>
@@ -45266,8 +45381,17 @@
       <c r="I179" t="s">
         <v>2655</v>
       </c>
-    </row>
-    <row r="180" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J179" t="s">
+        <v>3517</v>
+      </c>
+      <c r="K179" t="s">
+        <v>3487</v>
+      </c>
+      <c r="L179" t="s">
+        <v>3522</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>2965</v>
       </c>
@@ -45293,7 +45417,7 @@
         <v>2968</v>
       </c>
     </row>
-    <row r="181" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>2883</v>
       </c>
@@ -45321,8 +45445,17 @@
       <c r="I181" t="s">
         <v>2887</v>
       </c>
-    </row>
-    <row r="182" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J181" t="s">
+        <v>3517</v>
+      </c>
+      <c r="K181" t="s">
+        <v>3508</v>
+      </c>
+      <c r="L181" t="s">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>2755</v>
       </c>
@@ -45351,7 +45484,7 @@
         <v>2759</v>
       </c>
     </row>
-    <row r="183" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>1890</v>
       </c>
@@ -45380,7 +45513,7 @@
         <v>1894</v>
       </c>
     </row>
-    <row r="184" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>3378</v>
       </c>
@@ -45408,8 +45541,17 @@
       <c r="I184" t="s">
         <v>3382</v>
       </c>
-    </row>
-    <row r="185" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J184" t="s">
+        <v>3517</v>
+      </c>
+      <c r="K184" t="s">
+        <v>3486</v>
+      </c>
+      <c r="L184" t="s">
+        <v>3508</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>2773</v>
       </c>
@@ -45438,7 +45580,7 @@
         <v>2777</v>
       </c>
     </row>
-    <row r="186" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>1254</v>
       </c>
@@ -45467,7 +45609,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="187" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>2305</v>
       </c>
@@ -45493,7 +45635,7 @@
         <v>2308</v>
       </c>
     </row>
-    <row r="188" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>3256</v>
       </c>
@@ -45522,7 +45664,7 @@
         <v>3260</v>
       </c>
     </row>
-    <row r="189" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>2316</v>
       </c>
@@ -45551,7 +45693,7 @@
         <v>2320</v>
       </c>
     </row>
-    <row r="190" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>2696</v>
       </c>
@@ -45580,7 +45722,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="191" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>1120</v>
       </c>
@@ -45606,7 +45748,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="192" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>2874</v>
       </c>
@@ -46138,7 +46280,7 @@
         <v>2736</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>1238</v>
       </c>
@@ -46167,7 +46309,7 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="210" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>538</v>
       </c>
@@ -46196,7 +46338,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="211" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>1860</v>
       </c>
@@ -46225,7 +46367,7 @@
         <v>1864</v>
       </c>
     </row>
-    <row r="212" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>3261</v>
       </c>
@@ -46254,7 +46396,7 @@
         <v>3265</v>
       </c>
     </row>
-    <row r="213" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>3023</v>
       </c>
@@ -46282,8 +46424,17 @@
       <c r="I213" t="s">
         <v>3027</v>
       </c>
-    </row>
-    <row r="214" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J213" t="s">
+        <v>3505</v>
+      </c>
+      <c r="K213" t="s">
+        <v>3486</v>
+      </c>
+      <c r="L213" t="s">
+        <v>3519</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>2969</v>
       </c>
@@ -46312,7 +46463,7 @@
         <v>2973</v>
       </c>
     </row>
-    <row r="215" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>3247</v>
       </c>
@@ -46341,7 +46492,7 @@
         <v>3251</v>
       </c>
     </row>
-    <row r="216" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>2747</v>
       </c>
@@ -46370,7 +46521,7 @@
         <v>2750</v>
       </c>
     </row>
-    <row r="217" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>2710</v>
       </c>
@@ -46399,7 +46550,7 @@
         <v>2714</v>
       </c>
     </row>
-    <row r="218" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>2571</v>
       </c>
@@ -46428,7 +46579,7 @@
         <v>2574</v>
       </c>
     </row>
-    <row r="219" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>3215</v>
       </c>
@@ -46457,7 +46608,7 @@
         <v>3218</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>2126</v>
       </c>
@@ -46486,7 +46637,7 @@
         <v>2130</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>2879</v>
       </c>
@@ -46515,7 +46666,7 @@
         <v>2882</v>
       </c>
     </row>
-    <row r="222" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>3155</v>
       </c>
@@ -46544,7 +46695,7 @@
         <v>3159</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>3330</v>
       </c>
@@ -46572,8 +46723,17 @@
       <c r="I223" t="s">
         <v>3334</v>
       </c>
-    </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J223" t="s">
+        <v>3518</v>
+      </c>
+      <c r="K223" t="s">
+        <v>3508</v>
+      </c>
+      <c r="L223" t="s">
+        <v>3505</v>
+      </c>
+    </row>
+    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>2590</v>
       </c>
@@ -46601,8 +46761,17 @@
       <c r="I224" t="s">
         <v>2593</v>
       </c>
-    </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J224" t="s">
+        <v>3518</v>
+      </c>
+      <c r="K224" t="s">
+        <v>3508</v>
+      </c>
+      <c r="L224" t="s">
+        <v>3505</v>
+      </c>
+    </row>
+    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>3010</v>
       </c>
@@ -46630,8 +46799,17 @@
       <c r="I225" t="s">
         <v>3013</v>
       </c>
-    </row>
-    <row r="226" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J225" t="s">
+        <v>3518</v>
+      </c>
+      <c r="K225" t="s">
+        <v>3508</v>
+      </c>
+      <c r="L225" t="s">
+        <v>3503</v>
+      </c>
+    </row>
+    <row r="226" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>1022</v>
       </c>
@@ -46660,7 +46838,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="227" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>2176</v>
       </c>
@@ -46689,7 +46867,7 @@
         <v>2180</v>
       </c>
     </row>
-    <row r="228" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>2224</v>
       </c>
@@ -46718,7 +46896,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="229" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>353</v>
       </c>
@@ -46747,7 +46925,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>239</v>
       </c>
@@ -46776,7 +46954,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="231" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>1965</v>
       </c>
@@ -46805,7 +46983,7 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="232" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>1427</v>
       </c>
@@ -46834,7 +47012,7 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="233" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>949</v>
       </c>
@@ -46862,8 +47040,17 @@
       <c r="I233" t="s">
         <v>953</v>
       </c>
-    </row>
-    <row r="234" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J233" t="s">
+        <v>3487</v>
+      </c>
+      <c r="K233" t="s">
+        <v>3499</v>
+      </c>
+      <c r="L233" t="s">
+        <v>3532</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>949</v>
       </c>
@@ -46892,7 +47079,7 @@
         <v>1625</v>
       </c>
     </row>
-    <row r="235" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>2448</v>
       </c>
@@ -46918,7 +47105,7 @@
         <v>2451</v>
       </c>
     </row>
-    <row r="236" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>3433</v>
       </c>
@@ -46944,7 +47131,7 @@
         <v>3436</v>
       </c>
     </row>
-    <row r="237" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>1909</v>
       </c>
@@ -46970,7 +47157,7 @@
         <v>1912</v>
       </c>
     </row>
-    <row r="238" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>846</v>
       </c>
@@ -46999,7 +47186,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="239" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>984</v>
       </c>
@@ -47025,7 +47212,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="240" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>1692</v>
       </c>
@@ -47051,7 +47238,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="241" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>1155</v>
       </c>
@@ -47077,7 +47264,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="242" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>3296</v>
       </c>
@@ -47106,7 +47293,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="243" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>2821</v>
       </c>
@@ -47135,7 +47322,7 @@
         <v>2825</v>
       </c>
     </row>
-    <row r="244" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>1725</v>
       </c>
@@ -47164,7 +47351,7 @@
         <v>1729</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>934</v>
       </c>
@@ -47193,7 +47380,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="246" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>1138</v>
       </c>
@@ -47219,7 +47406,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="247" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>2055</v>
       </c>
@@ -47244,8 +47431,14 @@
       <c r="I247" t="s">
         <v>2058</v>
       </c>
-    </row>
-    <row r="248" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="J247" t="s">
+        <v>3486</v>
+      </c>
+      <c r="K247" t="s">
+        <v>3522</v>
+      </c>
+    </row>
+    <row r="248" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>1701</v>
       </c>
@@ -47274,7 +47467,7 @@
         <v>1705</v>
       </c>
     </row>
-    <row r="249" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>954</v>
       </c>
@@ -47300,7 +47493,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="250" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>1829</v>
       </c>
@@ -47326,7 +47519,7 @@
         <v>1832</v>
       </c>
     </row>
-    <row r="251" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>2368</v>
       </c>
@@ -47355,7 +47548,7 @@
         <v>2372</v>
       </c>
     </row>
-    <row r="252" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>3128</v>
       </c>
@@ -47384,7 +47577,7 @@
         <v>3132</v>
       </c>
     </row>
-    <row r="253" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>115</v>
       </c>
@@ -47413,7 +47606,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="254" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>1784</v>
       </c>
@@ -47439,7 +47632,7 @@
         <v>1787</v>
       </c>
     </row>
-    <row r="255" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>482</v>
       </c>
@@ -47468,7 +47661,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="256" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>2290</v>
       </c>
@@ -47492,6 +47685,15 @@
       </c>
       <c r="I256" t="s">
         <v>2293</v>
+      </c>
+      <c r="J256" t="s">
+        <v>3486</v>
+      </c>
+      <c r="K256" t="s">
+        <v>3516</v>
+      </c>
+      <c r="L256" t="s">
+        <v>3497</v>
       </c>
     </row>
     <row r="257" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -47638,6 +47840,15 @@
       <c r="I261" t="s">
         <v>1500</v>
       </c>
+      <c r="J261" t="s">
+        <v>3522</v>
+      </c>
+      <c r="K261" t="s">
+        <v>3486</v>
+      </c>
+      <c r="L261" t="s">
+        <v>3473</v>
+      </c>
     </row>
     <row r="262" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
@@ -47801,6 +48012,15 @@
       <c r="I266" t="s">
         <v>299</v>
       </c>
+      <c r="J266" t="s">
+        <v>3532</v>
+      </c>
+      <c r="K266" t="s">
+        <v>3494</v>
+      </c>
+      <c r="L266" t="s">
+        <v>3489</v>
+      </c>
     </row>
     <row r="267" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
@@ -49910,7 +50130,7 @@
         <v>3201</v>
       </c>
     </row>
-    <row r="337" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>1833</v>
       </c>
@@ -49938,8 +50158,17 @@
       <c r="I337" t="s">
         <v>1837</v>
       </c>
-    </row>
-    <row r="338" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="J337" t="s">
+        <v>3486</v>
+      </c>
+      <c r="K337" t="s">
+        <v>3522</v>
+      </c>
+      <c r="L337" t="s">
+        <v>3473</v>
+      </c>
+    </row>
+    <row r="338" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>2387</v>
       </c>
@@ -49968,7 +50197,7 @@
         <v>2391</v>
       </c>
     </row>
-    <row r="339" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>2196</v>
       </c>
@@ -49997,7 +50226,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="340" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>2408</v>
       </c>
@@ -50026,7 +50255,7 @@
         <v>2412</v>
       </c>
     </row>
-    <row r="341" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>1550</v>
       </c>
@@ -50055,7 +50284,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="342" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>3388</v>
       </c>
@@ -50084,7 +50313,7 @@
         <v>3392</v>
       </c>
     </row>
-    <row r="343" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>283</v>
       </c>
@@ -50113,7 +50342,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="344" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>283</v>
       </c>
@@ -50142,7 +50371,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="345" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>1581</v>
       </c>
@@ -50171,7 +50400,7 @@
         <v>1585</v>
       </c>
     </row>
-    <row r="346" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>2373</v>
       </c>
@@ -50197,7 +50426,7 @@
         <v>2376</v>
       </c>
     </row>
-    <row r="347" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>1008</v>
       </c>
@@ -50226,7 +50455,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="348" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>964</v>
       </c>
@@ -50255,7 +50484,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="349" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>964</v>
       </c>
@@ -50284,7 +50513,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="350" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>2905</v>
       </c>
@@ -50313,7 +50542,7 @@
         <v>2909</v>
       </c>
     </row>
-    <row r="351" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>2525</v>
       </c>
@@ -50342,7 +50571,7 @@
         <v>2529</v>
       </c>
     </row>
-    <row r="352" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>2233</v>
       </c>
@@ -50368,7 +50597,7 @@
         <v>2236</v>
       </c>
     </row>
-    <row r="353" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>154</v>
       </c>
@@ -50397,7 +50626,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="354" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>1151</v>
       </c>
@@ -50423,7 +50652,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="355" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>2073</v>
       </c>
@@ -50449,7 +50678,7 @@
         <v>2076</v>
       </c>
     </row>
-    <row r="356" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>2826</v>
       </c>
@@ -50478,7 +50707,7 @@
         <v>2830</v>
       </c>
     </row>
-    <row r="357" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>3168</v>
       </c>
@@ -50507,7 +50736,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="358" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>416</v>
       </c>
@@ -50533,7 +50762,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="359" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>801</v>
       </c>
@@ -50559,7 +50788,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="360" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>2109</v>
       </c>
@@ -50584,8 +50813,17 @@
       <c r="I360" t="s">
         <v>2112</v>
       </c>
-    </row>
-    <row r="361" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J360" t="s">
+        <v>3486</v>
+      </c>
+      <c r="K360" t="s">
+        <v>3522</v>
+      </c>
+      <c r="L360" t="s">
+        <v>3473</v>
+      </c>
+    </row>
+    <row r="361" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>2599</v>
       </c>
@@ -50614,7 +50852,7 @@
         <v>2603</v>
       </c>
     </row>
-    <row r="362" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>3164</v>
       </c>
@@ -50643,7 +50881,7 @@
         <v>3167</v>
       </c>
     </row>
-    <row r="363" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>2781</v>
       </c>
@@ -50669,7 +50907,7 @@
         <v>2784</v>
       </c>
     </row>
-    <row r="364" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>2453</v>
       </c>
@@ -50698,7 +50936,7 @@
         <v>2457</v>
       </c>
     </row>
-    <row r="365" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>1638</v>
       </c>
@@ -50726,8 +50964,17 @@
       <c r="I365" t="s">
         <v>1642</v>
       </c>
-    </row>
-    <row r="366" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J365" t="s">
+        <v>3508</v>
+      </c>
+      <c r="K365" t="s">
+        <v>3517</v>
+      </c>
+      <c r="L365" t="s">
+        <v>3503</v>
+      </c>
+    </row>
+    <row r="366" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>1086</v>
       </c>
@@ -50756,7 +51003,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="367" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>2838</v>
       </c>
@@ -50785,7 +51032,7 @@
         <v>2842</v>
       </c>
     </row>
-    <row r="368" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>3324</v>
       </c>
@@ -50812,6 +51059,15 @@
       </c>
       <c r="I368" t="s">
         <v>3328</v>
+      </c>
+      <c r="J368" t="s">
+        <v>3518</v>
+      </c>
+      <c r="K368" t="s">
+        <v>3486</v>
+      </c>
+      <c r="L368" t="s">
+        <v>3487</v>
       </c>
     </row>
     <row r="369" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -50839,6 +51095,15 @@
       <c r="I369" t="s">
         <v>2543</v>
       </c>
+      <c r="J369" t="s">
+        <v>3518</v>
+      </c>
+      <c r="K369" t="s">
+        <v>3522</v>
+      </c>
+      <c r="L369" t="s">
+        <v>3508</v>
+      </c>
     </row>
     <row r="370" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
@@ -50984,6 +51249,15 @@
       <c r="I374" t="s">
         <v>495</v>
       </c>
+      <c r="J374" t="s">
+        <v>3486</v>
+      </c>
+      <c r="K374" t="s">
+        <v>3522</v>
+      </c>
+      <c r="L374" t="s">
+        <v>3532</v>
+      </c>
     </row>
     <row r="375" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
@@ -51129,6 +51403,15 @@
       <c r="I379" t="s">
         <v>1393</v>
       </c>
+      <c r="J379" t="s">
+        <v>3487</v>
+      </c>
+      <c r="K379" t="s">
+        <v>3532</v>
+      </c>
+      <c r="L379" t="s">
+        <v>3514</v>
+      </c>
     </row>
     <row r="380" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
@@ -51196,6 +51479,15 @@
       <c r="I381" t="s">
         <v>62</v>
       </c>
+      <c r="J381" t="s">
+        <v>3487</v>
+      </c>
+      <c r="K381" t="s">
+        <v>3532</v>
+      </c>
+      <c r="L381" t="s">
+        <v>3514</v>
+      </c>
     </row>
     <row r="382" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
@@ -51284,7 +51576,7 @@
         <v>2084</v>
       </c>
     </row>
-    <row r="385" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>278</v>
       </c>
@@ -51313,7 +51605,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="386" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>2816</v>
       </c>
@@ -51339,7 +51631,7 @@
         <v>2819</v>
       </c>
     </row>
-    <row r="387" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>924</v>
       </c>
@@ -51368,7 +51660,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="388" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>524</v>
       </c>
@@ -51397,7 +51689,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="389" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>1115</v>
       </c>
@@ -51426,7 +51718,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="390" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>1400</v>
       </c>
@@ -51455,7 +51747,7 @@
         <v>1404</v>
       </c>
     </row>
-    <row r="391" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>2458</v>
       </c>
@@ -51484,7 +51776,7 @@
         <v>2462</v>
       </c>
     </row>
-    <row r="392" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>3042</v>
       </c>
@@ -51513,7 +51805,7 @@
         <v>3046</v>
       </c>
     </row>
-    <row r="393" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>2848</v>
       </c>
@@ -51542,7 +51834,7 @@
         <v>2852</v>
       </c>
     </row>
-    <row r="394" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>3353</v>
       </c>
@@ -51571,7 +51863,7 @@
         <v>3357</v>
       </c>
     </row>
-    <row r="395" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>1818</v>
       </c>
@@ -51600,7 +51892,7 @@
         <v>1822</v>
       </c>
     </row>
-    <row r="396" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>3052</v>
       </c>
@@ -51629,7 +51921,7 @@
         <v>3056</v>
       </c>
     </row>
-    <row r="397" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>2974</v>
       </c>
@@ -51657,8 +51949,17 @@
       <c r="I397" t="s">
         <v>2978</v>
       </c>
-    </row>
-    <row r="398" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J397" t="s">
+        <v>3517</v>
+      </c>
+      <c r="K397" t="s">
+        <v>3487</v>
+      </c>
+      <c r="L397" t="s">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="398" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>2511</v>
       </c>
@@ -51687,7 +51988,7 @@
         <v>2515</v>
       </c>
     </row>
-    <row r="399" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>3447</v>
       </c>
@@ -51716,7 +52017,7 @@
         <v>3450</v>
       </c>
     </row>
-    <row r="400" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>3123</v>
       </c>
@@ -51773,6 +52074,15 @@
       <c r="I401" t="s">
         <v>2704</v>
       </c>
+      <c r="J401" t="s">
+        <v>3517</v>
+      </c>
+      <c r="K401" t="s">
+        <v>3487</v>
+      </c>
+      <c r="L401" t="s">
+        <v>3518</v>
+      </c>
     </row>
     <row r="402" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
@@ -51860,6 +52170,15 @@
       <c r="I404" t="s">
         <v>3005</v>
       </c>
+      <c r="J404" t="s">
+        <v>3517</v>
+      </c>
+      <c r="K404" t="s">
+        <v>3487</v>
+      </c>
+      <c r="L404" t="s">
+        <v>3518</v>
+      </c>
     </row>
     <row r="405" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
@@ -52635,6 +52954,15 @@
       <c r="I427" t="s">
         <v>2768</v>
       </c>
+      <c r="J427" t="s">
+        <v>3508</v>
+      </c>
+      <c r="K427" t="s">
+        <v>3503</v>
+      </c>
+      <c r="L427" t="s">
+        <v>3505</v>
+      </c>
     </row>
     <row r="428" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
@@ -52870,6 +53198,15 @@
       <c r="I435" t="s">
         <v>1305</v>
       </c>
+      <c r="J435" t="s">
+        <v>3486</v>
+      </c>
+      <c r="K435" t="s">
+        <v>3532</v>
+      </c>
+      <c r="L435" t="s">
+        <v>3534</v>
+      </c>
     </row>
     <row r="436" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
@@ -53076,6 +53413,15 @@
       <c r="I442" t="s">
         <v>1137</v>
       </c>
+      <c r="J442" t="s">
+        <v>3487</v>
+      </c>
+      <c r="K442" t="s">
+        <v>3516</v>
+      </c>
+      <c r="L442" t="s">
+        <v>3497</v>
+      </c>
     </row>
     <row r="443" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
@@ -53257,7 +53603,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="449" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>1046</v>
       </c>
@@ -53286,7 +53632,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="450" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>3437</v>
       </c>
@@ -53315,7 +53661,7 @@
         <v>3440</v>
       </c>
     </row>
-    <row r="451" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>2049</v>
       </c>
@@ -53344,7 +53690,7 @@
         <v>2053</v>
       </c>
     </row>
-    <row r="452" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>2121</v>
       </c>
@@ -53373,7 +53719,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="453" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>1332</v>
       </c>
@@ -53398,8 +53744,17 @@
       <c r="I453" t="s">
         <v>1335</v>
       </c>
-    </row>
-    <row r="454" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J453" t="s">
+        <v>3497</v>
+      </c>
+      <c r="K453" t="s">
+        <v>3532</v>
+      </c>
+      <c r="L453" t="s">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="454" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>1091</v>
       </c>
@@ -53428,7 +53783,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="455" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
         <v>988</v>
       </c>
@@ -53457,7 +53812,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="456" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
         <v>2685</v>
       </c>
@@ -53486,7 +53841,7 @@
         <v>2688</v>
       </c>
     </row>
-    <row r="457" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
         <v>1666</v>
       </c>
@@ -53515,7 +53870,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="458" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>1357</v>
       </c>
@@ -53541,7 +53896,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="459" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
         <v>2353</v>
       </c>
@@ -53567,7 +53922,7 @@
         <v>2356</v>
       </c>
     </row>
-    <row r="460" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
         <v>2737</v>
       </c>
@@ -53596,7 +53951,7 @@
         <v>2741</v>
       </c>
     </row>
-    <row r="461" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
         <v>1843</v>
       </c>
@@ -53625,7 +53980,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="462" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
         <v>1502</v>
       </c>
@@ -53654,7 +54009,7 @@
         <v>1505</v>
       </c>
     </row>
-    <row r="463" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>914</v>
       </c>
@@ -53683,7 +54038,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="464" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
         <v>1437</v>
       </c>
@@ -53709,7 +54064,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="465" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
         <v>1823</v>
       </c>
@@ -53738,7 +54093,7 @@
         <v>1827</v>
       </c>
     </row>
-    <row r="466" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
         <v>1406</v>
       </c>
@@ -53766,8 +54121,17 @@
       <c r="I466" t="s">
         <v>1410</v>
       </c>
-    </row>
-    <row r="467" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J466" t="s">
+        <v>3522</v>
+      </c>
+      <c r="K466" t="s">
+        <v>3532</v>
+      </c>
+      <c r="L466" t="s">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="467" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
         <v>3266</v>
       </c>
@@ -53796,7 +54160,7 @@
         <v>3270</v>
       </c>
     </row>
-    <row r="468" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
         <v>2263</v>
       </c>
@@ -53822,7 +54186,7 @@
         <v>2266</v>
       </c>
     </row>
-    <row r="469" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
         <v>3456</v>
       </c>
@@ -53848,7 +54212,7 @@
         <v>3459</v>
       </c>
     </row>
-    <row r="470" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
         <v>2961</v>
       </c>
@@ -53874,7 +54238,7 @@
         <v>2964</v>
       </c>
     </row>
-    <row r="471" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
         <v>1066</v>
       </c>
@@ -53903,7 +54267,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="472" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
         <v>95</v>
       </c>
@@ -53932,7 +54296,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="473" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
         <v>95</v>
       </c>
@@ -53961,7 +54325,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="474" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
         <v>1178</v>
       </c>
@@ -53990,7 +54354,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="475" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
         <v>159</v>
       </c>
@@ -54019,7 +54383,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="476" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>1456</v>
       </c>
@@ -54048,7 +54412,7 @@
         <v>1460</v>
       </c>
     </row>
-    <row r="477" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
         <v>939</v>
       </c>
@@ -54077,7 +54441,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="478" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
         <v>1384</v>
       </c>
@@ -54102,8 +54466,17 @@
       <c r="I478" t="s">
         <v>1387</v>
       </c>
-    </row>
-    <row r="479" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="J478" t="s">
+        <v>3514</v>
+      </c>
+      <c r="K478" t="s">
+        <v>3487</v>
+      </c>
+      <c r="L478" t="s">
+        <v>3493</v>
+      </c>
+    </row>
+    <row r="479" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
         <v>2705</v>
       </c>
@@ -54132,7 +54505,7 @@
         <v>2709</v>
       </c>
     </row>
-    <row r="480" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
         <v>1517</v>
       </c>
@@ -54158,7 +54531,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="481" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
         <v>851</v>
       </c>
@@ -54187,7 +54560,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="482" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
         <v>472</v>
       </c>
@@ -54216,7 +54589,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="483" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
         <v>2346</v>
       </c>
@@ -54245,7 +54618,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="484" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
         <v>1395</v>
       </c>
@@ -54274,7 +54647,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="485" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
         <v>3211</v>
       </c>
@@ -54300,7 +54673,7 @@
         <v>3214</v>
       </c>
     </row>
-    <row r="486" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
         <v>1071</v>
       </c>
@@ -54329,7 +54702,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="487" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
         <v>2580</v>
       </c>
@@ -54358,7 +54731,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="488" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
         <v>2580</v>
       </c>
@@ -54386,8 +54759,17 @@
       <c r="I488" t="s">
         <v>2584</v>
       </c>
-    </row>
-    <row r="489" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J488" t="s">
+        <v>3505</v>
+      </c>
+      <c r="K488" t="s">
+        <v>3518</v>
+      </c>
+      <c r="L488" t="s">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="489" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
         <v>616</v>
       </c>
@@ -54416,7 +54798,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="490" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
         <v>1587</v>
       </c>
@@ -54445,7 +54827,7 @@
         <v>1591</v>
       </c>
     </row>
-    <row r="491" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
         <v>826</v>
       </c>
@@ -54473,8 +54855,17 @@
       <c r="I491" t="s">
         <v>830</v>
       </c>
-    </row>
-    <row r="492" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J491" t="s">
+        <v>3505</v>
+      </c>
+      <c r="K491" t="s">
+        <v>3486</v>
+      </c>
+      <c r="L491" t="s">
+        <v>3493</v>
+      </c>
+    </row>
+    <row r="492" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
         <v>364</v>
       </c>
@@ -54503,7 +54894,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="493" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
         <v>580</v>
       </c>
@@ -54532,7 +54923,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="494" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
         <v>580</v>
       </c>
@@ -54561,7 +54952,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="495" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
         <v>301</v>
       </c>
@@ -54590,7 +54981,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="496" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
         <v>993</v>
       </c>
@@ -54619,7 +55010,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="497" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
         <v>179</v>
       </c>
@@ -54645,7 +55036,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="498" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
         <v>496</v>
       </c>
@@ -54671,7 +55062,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="499" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
         <v>897</v>
       </c>
@@ -54697,7 +55088,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="500" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
         <v>2085</v>
       </c>
@@ -54726,7 +55117,7 @@
         <v>2089</v>
       </c>
     </row>
-    <row r="501" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
         <v>1990</v>
       </c>
@@ -54754,8 +55145,17 @@
       <c r="I501" t="s">
         <v>1994</v>
       </c>
-    </row>
-    <row r="502" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J501" t="s">
+        <v>3487</v>
+      </c>
+      <c r="K501" t="s">
+        <v>3522</v>
+      </c>
+      <c r="L501" t="s">
+        <v>3532</v>
+      </c>
+    </row>
+    <row r="502" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
         <v>3409</v>
       </c>
@@ -54784,7 +55184,7 @@
         <v>3413</v>
       </c>
     </row>
-    <row r="503" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
         <v>2494</v>
       </c>
@@ -54813,7 +55213,7 @@
         <v>2498</v>
       </c>
     </row>
-    <row r="504" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
         <v>2559</v>
       </c>
@@ -54842,7 +55242,7 @@
         <v>2563</v>
       </c>
     </row>
-    <row r="505" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
         <v>3398</v>
       </c>
@@ -54871,7 +55271,7 @@
         <v>3402</v>
       </c>
     </row>
-    <row r="506" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
         <v>3160</v>
       </c>
@@ -54900,7 +55300,7 @@
         <v>3163</v>
       </c>
     </row>
-    <row r="507" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
         <v>3099</v>
       </c>
@@ -54929,7 +55329,7 @@
         <v>3103</v>
       </c>
     </row>
-    <row r="508" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
         <v>3135</v>
       </c>
@@ -54958,7 +55358,7 @@
         <v>3139</v>
       </c>
     </row>
-    <row r="509" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
         <v>3178</v>
       </c>
@@ -54987,7 +55387,7 @@
         <v>3182</v>
       </c>
     </row>
-    <row r="510" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
         <v>2864</v>
       </c>
@@ -55016,7 +55416,7 @@
         <v>2867</v>
       </c>
     </row>
-    <row r="511" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
         <v>3145</v>
       </c>
@@ -55044,8 +55444,17 @@
       <c r="I511" t="s">
         <v>3149</v>
       </c>
-    </row>
-    <row r="512" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J511" t="s">
+        <v>3487</v>
+      </c>
+      <c r="K511" t="s">
+        <v>3518</v>
+      </c>
+      <c r="L511" t="s">
+        <v>3503</v>
+      </c>
+    </row>
+    <row r="512" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
         <v>3405</v>
       </c>
@@ -55071,7 +55480,7 @@
         <v>3408</v>
       </c>
     </row>
-    <row r="513" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
         <v>2403</v>
       </c>
@@ -55100,7 +55509,7 @@
         <v>2407</v>
       </c>
     </row>
-    <row r="514" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
         <v>1555</v>
       </c>
@@ -55126,7 +55535,7 @@
         <v>1558</v>
       </c>
     </row>
-    <row r="515" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
         <v>2630</v>
       </c>
@@ -55155,7 +55564,7 @@
         <v>2634</v>
       </c>
     </row>
-    <row r="516" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
         <v>1813</v>
       </c>
@@ -55184,7 +55593,7 @@
         <v>1817</v>
       </c>
     </row>
-    <row r="517" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
         <v>2005</v>
       </c>
@@ -55213,7 +55622,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="518" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
         <v>1507</v>
       </c>
@@ -55242,7 +55651,7 @@
         <v>1511</v>
       </c>
     </row>
-    <row r="519" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
         <v>567</v>
       </c>
@@ -55268,7 +55677,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="520" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
         <v>2676</v>
       </c>
@@ -55296,8 +55705,17 @@
       <c r="I520" t="s">
         <v>2680</v>
       </c>
-    </row>
-    <row r="521" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J520" t="s">
+        <v>3522</v>
+      </c>
+      <c r="K520" t="s">
+        <v>3487</v>
+      </c>
+      <c r="L520" t="s">
+        <v>3499</v>
+      </c>
+    </row>
+    <row r="521" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
         <v>3071</v>
       </c>
@@ -55326,7 +55744,7 @@
         <v>3075</v>
       </c>
     </row>
-    <row r="522" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
         <v>708</v>
       </c>
@@ -55355,7 +55773,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="523" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
         <v>929</v>
       </c>
@@ -55384,7 +55802,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="524" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
         <v>1708</v>
       </c>
@@ -55410,7 +55828,7 @@
         <v>1711</v>
       </c>
     </row>
-    <row r="525" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
         <v>2393</v>
       </c>
@@ -55439,7 +55857,7 @@
         <v>2397</v>
       </c>
     </row>
-    <row r="526" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
         <v>1286</v>
       </c>
@@ -55468,7 +55886,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="527" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
         <v>1568</v>
       </c>
@@ -55494,7 +55912,7 @@
         <v>1571</v>
       </c>
     </row>
-    <row r="528" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
         <v>1036</v>
       </c>
@@ -55523,7 +55941,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="529" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
         <v>84</v>
       </c>
@@ -55552,7 +55970,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="530" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
         <v>841</v>
       </c>
@@ -55581,7 +55999,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="531" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
         <v>760</v>
       </c>
@@ -55607,7 +56025,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="532" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
         <v>2148</v>
       </c>
@@ -55636,7 +56054,7 @@
         <v>2152</v>
       </c>
     </row>
-    <row r="533" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
         <v>1096</v>
       </c>
@@ -55665,7 +56083,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="534" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
         <v>2499</v>
       </c>
@@ -55693,8 +56111,17 @@
       <c r="I534" t="s">
         <v>2503</v>
       </c>
-    </row>
-    <row r="535" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J534" t="s">
+        <v>3487</v>
+      </c>
+      <c r="K534" t="s">
+        <v>3522</v>
+      </c>
+      <c r="L534" t="s">
+        <v>3494</v>
+      </c>
+    </row>
+    <row r="535" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
         <v>1546</v>
       </c>
@@ -55720,7 +56147,7 @@
         <v>1549</v>
       </c>
     </row>
-    <row r="536" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
         <v>3335</v>
       </c>
@@ -55746,7 +56173,7 @@
         <v>3338</v>
       </c>
     </row>
-    <row r="537" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
         <v>3416</v>
       </c>
@@ -55772,7 +56199,7 @@
         <v>3419</v>
       </c>
     </row>
-    <row r="538" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
         <v>1920</v>
       </c>
@@ -55798,7 +56225,7 @@
         <v>1923</v>
       </c>
     </row>
-    <row r="539" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
         <v>14</v>
       </c>
@@ -55824,7 +56251,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="540" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="540" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
         <v>1915</v>
       </c>
@@ -55853,7 +56280,7 @@
         <v>1919</v>
       </c>
     </row>
-    <row r="541" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="541" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
         <v>2544</v>
       </c>
@@ -55882,7 +56309,7 @@
         <v>2548</v>
       </c>
     </row>
-    <row r="542" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="542" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
         <v>2000</v>
       </c>
@@ -55911,7 +56338,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="543" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="543" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A543" t="s">
         <v>2191</v>
       </c>
@@ -55940,7 +56367,7 @@
         <v>2195</v>
       </c>
     </row>
-    <row r="544" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A544" t="s">
         <v>1947</v>
       </c>
@@ -55968,8 +56395,17 @@
       <c r="I544" t="s">
         <v>1951</v>
       </c>
-    </row>
-    <row r="545" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="J544" t="s">
+        <v>3497</v>
+      </c>
+      <c r="K544" t="s">
+        <v>3486</v>
+      </c>
+      <c r="L544" t="s">
+        <v>3532</v>
+      </c>
+    </row>
+    <row r="545" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
         <v>2893</v>
       </c>
@@ -55998,7 +56434,7 @@
         <v>2897</v>
       </c>
     </row>
-    <row r="546" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="546" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
         <v>3304</v>
       </c>
@@ -56024,7 +56460,7 @@
         <v>3307</v>
       </c>
     </row>
-    <row r="547" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
         <v>19</v>
       </c>
@@ -56053,7 +56489,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="548" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="548" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A548" t="s">
         <v>739</v>
       </c>
@@ -56082,7 +56518,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="549" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="549" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
         <v>2565</v>
       </c>
@@ -56111,7 +56547,7 @@
         <v>2569</v>
       </c>
     </row>
-    <row r="550" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="550" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
         <v>3193</v>
       </c>
@@ -56140,7 +56576,7 @@
         <v>3197</v>
       </c>
     </row>
-    <row r="551" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="551" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A551" t="s">
         <v>411</v>
       </c>
@@ -56169,7 +56605,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="552" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="552" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A552" t="s">
         <v>1643</v>
       </c>
@@ -56197,8 +56633,17 @@
       <c r="I552" t="s">
         <v>1647</v>
       </c>
-    </row>
-    <row r="553" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J552" t="s">
+        <v>3487</v>
+      </c>
+      <c r="K552" t="s">
+        <v>3497</v>
+      </c>
+      <c r="L552" t="s">
+        <v>3532</v>
+      </c>
+    </row>
+    <row r="553" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
         <v>74</v>
       </c>
@@ -56227,7 +56672,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="554" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="554" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A554" t="s">
         <v>347</v>
       </c>
@@ -56256,7 +56701,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="555" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
         <v>1655</v>
       </c>
@@ -56285,7 +56730,7 @@
         <v>1659</v>
       </c>
     </row>
-    <row r="556" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="556" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A556" t="s">
         <v>1469</v>
       </c>
@@ -56314,7 +56759,7 @@
         <v>1473</v>
       </c>
     </row>
-    <row r="557" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="557" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
         <v>611</v>
       </c>
@@ -56343,7 +56788,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="558" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="558" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A558" t="s">
         <v>2068</v>
       </c>
@@ -56372,7 +56817,7 @@
         <v>2072</v>
       </c>
     </row>
-    <row r="559" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="559" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
         <v>245</v>
       </c>
@@ -56401,7 +56846,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="560" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="560" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
         <v>749</v>
       </c>
@@ -56650,6 +57095,15 @@
       <c r="I567" t="s">
         <v>3469</v>
       </c>
+      <c r="J567" t="s">
+        <v>3508</v>
+      </c>
+      <c r="K567" t="s">
+        <v>3503</v>
+      </c>
+      <c r="L567" t="s">
+        <v>3517</v>
+      </c>
     </row>
     <row r="568" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A568" t="s">
@@ -56921,7 +57375,7 @@
         <v>3516</v>
       </c>
     </row>
-    <row r="577" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="577" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A577" t="s">
         <v>233</v>
       </c>
@@ -56950,7 +57404,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="578" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="578" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A578" t="s">
         <v>2919</v>
       </c>
@@ -56976,7 +57430,7 @@
         <v>2922</v>
       </c>
     </row>
-    <row r="579" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="579" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A579" t="s">
         <v>1872</v>
       </c>
@@ -57002,7 +57456,7 @@
         <v>1875</v>
       </c>
     </row>
-    <row r="580" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="580" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A580" t="s">
         <v>2143</v>
       </c>
@@ -57031,7 +57485,7 @@
         <v>2147</v>
       </c>
     </row>
-    <row r="581" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="581" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
         <v>2030</v>
       </c>
@@ -57060,7 +57514,7 @@
         <v>2034</v>
       </c>
     </row>
-    <row r="582" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="582" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A582" t="s">
         <v>1146</v>
       </c>
@@ -57089,7 +57543,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="583" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="583" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
         <v>2899</v>
       </c>
@@ -57117,8 +57571,17 @@
       <c r="I583" t="s">
         <v>2903</v>
       </c>
-    </row>
-    <row r="584" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J583" t="s">
+        <v>3503</v>
+      </c>
+      <c r="K583" t="s">
+        <v>3486</v>
+      </c>
+      <c r="L583" t="s">
+        <v>3487</v>
+      </c>
+    </row>
+    <row r="584" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A584" t="s">
         <v>816</v>
       </c>
@@ -57147,7 +57610,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="585" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="585" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A585" t="s">
         <v>1937</v>
       </c>
@@ -57176,7 +57639,7 @@
         <v>1941</v>
       </c>
     </row>
-    <row r="586" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="586" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
         <v>892</v>
       </c>
@@ -57205,7 +57668,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="587" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="587" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A587" t="s">
         <v>1210</v>
       </c>
@@ -57231,7 +57694,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="588" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="588" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A588" t="s">
         <v>1954</v>
       </c>
@@ -57260,7 +57723,7 @@
         <v>1958</v>
       </c>
     </row>
-    <row r="589" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="589" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A589" t="s">
         <v>53</v>
       </c>
@@ -57289,7 +57752,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="590" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="590" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
         <v>877</v>
       </c>
@@ -57315,7 +57778,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="591" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="591" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A591" t="s">
         <v>3349</v>
       </c>
@@ -57344,7 +57807,7 @@
         <v>3352</v>
       </c>
     </row>
-    <row r="592" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="592" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A592" t="s">
         <v>1866</v>
       </c>
@@ -57601,6 +58064,12 @@
       <c r="I600" t="s">
         <v>2339</v>
       </c>
+      <c r="J600" t="s">
+        <v>3487</v>
+      </c>
+      <c r="K600" t="s">
+        <v>3481</v>
+      </c>
     </row>
     <row r="601" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A601" t="s">
@@ -58358,6 +58827,15 @@
       <c r="I626" t="s">
         <v>1946</v>
       </c>
+      <c r="J626" t="s">
+        <v>3506</v>
+      </c>
+      <c r="K626" t="s">
+        <v>3487</v>
+      </c>
+      <c r="L626" t="s">
+        <v>3514</v>
+      </c>
     </row>
     <row r="627" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A627" t="s">
@@ -59934,6 +60412,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L681" xr:uid="{84173DE9-3815-4818-B963-E90EED192D50}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding additional data and adjusting tagging algorithm
</commit_message>
<xml_diff>
--- a/app/Data/raw_data/manual_game_tagging.xlsx
+++ b/app/Data/raw_data/manual_game_tagging.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seelc\OneDrive\Desktop\Lucas Desktop Items\Projects\optigame_simple\optigame_simple\app\Data\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2ECBF4-E1B9-4C6D-9082-1B5F23DFF285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315DD373-28C9-4E89-8459-1EFF89042A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{237F2DA4-652B-41E0-AEDA-F9274CD289A5}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9767" uniqueCount="3535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9860" uniqueCount="3535">
   <si>
     <t>id</t>
   </si>
@@ -39827,8 +39827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80090C68-1AA8-4D07-8B4A-954A981011F1}">
   <dimension ref="A1:A59"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40137,8 +40137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84173DE9-3815-4818-B963-E90EED192D50}">
   <dimension ref="A1:L680"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A386" workbookViewId="0">
-      <selection activeCell="M386" sqref="M386"/>
+    <sheetView tabSelected="1" topLeftCell="A596" workbookViewId="0">
+      <selection activeCell="Q607" sqref="Q607"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52527,6 +52527,15 @@
       <c r="I404" t="s">
         <v>378</v>
       </c>
+      <c r="J404" t="s">
+        <v>3486</v>
+      </c>
+      <c r="K404" t="s">
+        <v>3490</v>
+      </c>
+      <c r="L404" t="s">
+        <v>3532</v>
+      </c>
     </row>
     <row r="405" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
@@ -53090,6 +53099,15 @@
       <c r="I420" t="s">
         <v>1218</v>
       </c>
+      <c r="J420" t="s">
+        <v>3532</v>
+      </c>
+      <c r="K420" t="s">
+        <v>3497</v>
+      </c>
+      <c r="L420" t="s">
+        <v>3487</v>
+      </c>
     </row>
     <row r="421" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
@@ -53148,6 +53166,15 @@
       <c r="I422" t="s">
         <v>2442</v>
       </c>
+      <c r="J422" t="s">
+        <v>3486</v>
+      </c>
+      <c r="K422" t="s">
+        <v>3517</v>
+      </c>
+      <c r="L422" t="s">
+        <v>3481</v>
+      </c>
     </row>
     <row r="423" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
@@ -53433,6 +53460,15 @@
       <c r="I431" t="s">
         <v>1540</v>
       </c>
+      <c r="J431" t="s">
+        <v>3532</v>
+      </c>
+      <c r="K431" t="s">
+        <v>3514</v>
+      </c>
+      <c r="L431" t="s">
+        <v>3487</v>
+      </c>
     </row>
     <row r="432" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
@@ -53703,6 +53739,15 @@
       <c r="I440" t="s">
         <v>109</v>
       </c>
+      <c r="J440" t="s">
+        <v>3487</v>
+      </c>
+      <c r="K440" t="s">
+        <v>3522</v>
+      </c>
+      <c r="L440" t="s">
+        <v>3532</v>
+      </c>
     </row>
     <row r="441" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
@@ -53825,6 +53870,15 @@
       <c r="I444" t="s">
         <v>1767</v>
       </c>
+      <c r="J444" t="s">
+        <v>3522</v>
+      </c>
+      <c r="K444" t="s">
+        <v>3487</v>
+      </c>
+      <c r="L444" t="s">
+        <v>3532</v>
+      </c>
     </row>
     <row r="445" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
@@ -53950,6 +54004,15 @@
       <c r="I448" t="s">
         <v>1050</v>
       </c>
+      <c r="J448" t="s">
+        <v>3532</v>
+      </c>
+      <c r="K448" t="s">
+        <v>3486</v>
+      </c>
+      <c r="L448" t="s">
+        <v>3514</v>
+      </c>
     </row>
     <row r="449" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
@@ -54240,6 +54303,15 @@
       <c r="I458" t="s">
         <v>2356</v>
       </c>
+      <c r="J458" t="s">
+        <v>3532</v>
+      </c>
+      <c r="K458" t="s">
+        <v>3487</v>
+      </c>
+      <c r="L458" t="s">
+        <v>3514</v>
+      </c>
     </row>
     <row r="459" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
@@ -54356,6 +54428,15 @@
       <c r="I462" t="s">
         <v>918</v>
       </c>
+      <c r="J462" t="s">
+        <v>3490</v>
+      </c>
+      <c r="K462" t="s">
+        <v>3487</v>
+      </c>
+      <c r="L462" t="s">
+        <v>3522</v>
+      </c>
     </row>
     <row r="463" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
@@ -54643,6 +54724,15 @@
       <c r="I472" t="s">
         <v>99</v>
       </c>
+      <c r="J472" t="s">
+        <v>3522</v>
+      </c>
+      <c r="K472" t="s">
+        <v>3486</v>
+      </c>
+      <c r="L472" t="s">
+        <v>3491</v>
+      </c>
     </row>
     <row r="473" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
@@ -54759,6 +54849,15 @@
       <c r="I476" t="s">
         <v>943</v>
       </c>
+      <c r="J476" t="s">
+        <v>3490</v>
+      </c>
+      <c r="K476" t="s">
+        <v>3532</v>
+      </c>
+      <c r="L476" t="s">
+        <v>3522</v>
+      </c>
     </row>
     <row r="477" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
@@ -54878,6 +54977,15 @@
       <c r="I480" t="s">
         <v>855</v>
       </c>
+      <c r="J480" t="s">
+        <v>3499</v>
+      </c>
+      <c r="K480" t="s">
+        <v>3532</v>
+      </c>
+      <c r="L480" t="s">
+        <v>3514</v>
+      </c>
     </row>
     <row r="481" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
@@ -55270,6 +55378,15 @@
       <c r="I493" t="s">
         <v>584</v>
       </c>
+      <c r="J493" t="s">
+        <v>3486</v>
+      </c>
+      <c r="K493" t="s">
+        <v>3481</v>
+      </c>
+      <c r="L493" t="s">
+        <v>3522</v>
+      </c>
     </row>
     <row r="494" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
@@ -55354,6 +55471,15 @@
       <c r="I496" t="s">
         <v>182</v>
       </c>
+      <c r="J496" t="s">
+        <v>3486</v>
+      </c>
+      <c r="K496" t="s">
+        <v>3522</v>
+      </c>
+      <c r="L496" t="s">
+        <v>3491</v>
+      </c>
     </row>
     <row r="497" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
@@ -55827,6 +55953,15 @@
       <c r="I512" t="s">
         <v>2407</v>
       </c>
+      <c r="J512" t="s">
+        <v>3487</v>
+      </c>
+      <c r="K512" t="s">
+        <v>3532</v>
+      </c>
+      <c r="L512" t="s">
+        <v>3491</v>
+      </c>
     </row>
     <row r="513" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
@@ -55969,6 +56104,15 @@
       <c r="I517" t="s">
         <v>1511</v>
       </c>
+      <c r="J517" t="s">
+        <v>3489</v>
+      </c>
+      <c r="K517" t="s">
+        <v>3490</v>
+      </c>
+      <c r="L517" t="s">
+        <v>3522</v>
+      </c>
     </row>
     <row r="518" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
@@ -56146,6 +56290,15 @@
       <c r="I523" t="s">
         <v>1711</v>
       </c>
+      <c r="J523" t="s">
+        <v>3497</v>
+      </c>
+      <c r="K523" t="s">
+        <v>3522</v>
+      </c>
+      <c r="L523" t="s">
+        <v>3486</v>
+      </c>
     </row>
     <row r="524" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
@@ -56259,6 +56412,15 @@
       <c r="I527" t="s">
         <v>1040</v>
       </c>
+      <c r="J527" t="s">
+        <v>3522</v>
+      </c>
+      <c r="K527" t="s">
+        <v>3486</v>
+      </c>
+      <c r="L527" t="s">
+        <v>3487</v>
+      </c>
     </row>
     <row r="528" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
@@ -56288,6 +56450,15 @@
       <c r="I528" t="s">
         <v>89</v>
       </c>
+      <c r="J528" t="s">
+        <v>3522</v>
+      </c>
+      <c r="K528" t="s">
+        <v>3486</v>
+      </c>
+      <c r="L528" t="s">
+        <v>3487</v>
+      </c>
     </row>
     <row r="529" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
@@ -56569,6 +56740,15 @@
       <c r="I538" t="s">
         <v>18</v>
       </c>
+      <c r="J538" t="s">
+        <v>3487</v>
+      </c>
+      <c r="K538" t="s">
+        <v>3499</v>
+      </c>
+      <c r="L538" t="s">
+        <v>3532</v>
+      </c>
     </row>
     <row r="539" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
@@ -56656,6 +56836,15 @@
       <c r="I541" t="s">
         <v>2004</v>
       </c>
+      <c r="J541" t="s">
+        <v>3487</v>
+      </c>
+      <c r="K541" t="s">
+        <v>3532</v>
+      </c>
+      <c r="L541" t="s">
+        <v>3497</v>
+      </c>
     </row>
     <row r="542" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
@@ -56807,6 +56996,15 @@
       <c r="I546" t="s">
         <v>24</v>
       </c>
+      <c r="J546" t="s">
+        <v>3489</v>
+      </c>
+      <c r="K546" t="s">
+        <v>3522</v>
+      </c>
+      <c r="L546" t="s">
+        <v>3486</v>
+      </c>
     </row>
     <row r="547" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
@@ -56865,6 +57063,15 @@
       <c r="I548" t="s">
         <v>2569</v>
       </c>
+      <c r="J548" t="s">
+        <v>3517</v>
+      </c>
+      <c r="K548" t="s">
+        <v>3518</v>
+      </c>
+      <c r="L548" t="s">
+        <v>3486</v>
+      </c>
     </row>
     <row r="549" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
@@ -57106,6 +57313,15 @@
       <c r="I556" t="s">
         <v>615</v>
       </c>
+      <c r="J556" t="s">
+        <v>3522</v>
+      </c>
+      <c r="K556" t="s">
+        <v>3523</v>
+      </c>
+      <c r="L556" t="s">
+        <v>3532</v>
+      </c>
     </row>
     <row r="557" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
@@ -57164,6 +57380,15 @@
       <c r="I558" t="s">
         <v>249</v>
       </c>
+      <c r="J558" t="s">
+        <v>3487</v>
+      </c>
+      <c r="K558" t="s">
+        <v>3516</v>
+      </c>
+      <c r="L558" t="s">
+        <v>3497</v>
+      </c>
     </row>
     <row r="559" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
@@ -57986,6 +58211,15 @@
       <c r="I585" t="s">
         <v>896</v>
       </c>
+      <c r="J585" t="s">
+        <v>3487</v>
+      </c>
+      <c r="K585" t="s">
+        <v>3514</v>
+      </c>
+      <c r="L585" t="s">
+        <v>3522</v>
+      </c>
     </row>
     <row r="586" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
@@ -58183,6 +58417,15 @@
       <c r="I592" t="s">
         <v>748</v>
       </c>
+      <c r="J592" t="s">
+        <v>3487</v>
+      </c>
+      <c r="K592" t="s">
+        <v>3514</v>
+      </c>
+      <c r="L592" t="s">
+        <v>3489</v>
+      </c>
     </row>
     <row r="593" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A593" t="s">
@@ -58212,6 +58455,15 @@
       <c r="I593" t="s">
         <v>336</v>
       </c>
+      <c r="J593" t="s">
+        <v>3487</v>
+      </c>
+      <c r="K593" t="s">
+        <v>3514</v>
+      </c>
+      <c r="L593" t="s">
+        <v>3489</v>
+      </c>
     </row>
     <row r="594" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A594" t="s">
@@ -58447,6 +58699,15 @@
       <c r="I601" t="s">
         <v>2493</v>
       </c>
+      <c r="J601" t="s">
+        <v>3486</v>
+      </c>
+      <c r="K601" t="s">
+        <v>3481</v>
+      </c>
+      <c r="L601" t="s">
+        <v>3517</v>
+      </c>
     </row>
     <row r="602" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A602" t="s">
@@ -58656,8 +58917,17 @@
       <c r="I608" t="s">
         <v>2815</v>
       </c>
-    </row>
-    <row r="609" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J608" t="s">
+        <v>3481</v>
+      </c>
+      <c r="K608" t="s">
+        <v>3486</v>
+      </c>
+      <c r="L608" t="s">
+        <v>3508</v>
+      </c>
+    </row>
+    <row r="609" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A609" t="s">
         <v>3373</v>
       </c>
@@ -58685,8 +58955,17 @@
       <c r="I609" t="s">
         <v>3377</v>
       </c>
-    </row>
-    <row r="610" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J609" t="s">
+        <v>3503</v>
+      </c>
+      <c r="K609" t="s">
+        <v>3481</v>
+      </c>
+      <c r="L609" t="s">
+        <v>3508</v>
+      </c>
+    </row>
+    <row r="610" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A610" t="s">
         <v>1778</v>
       </c>
@@ -58715,7 +58994,7 @@
         <v>1782</v>
       </c>
     </row>
-    <row r="611" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="611" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A611" t="s">
         <v>359</v>
       </c>
@@ -58744,7 +59023,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="612" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="612" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A612" t="s">
         <v>2843</v>
       </c>
@@ -58773,7 +59052,7 @@
         <v>2846</v>
       </c>
     </row>
-    <row r="613" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="613" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A613" t="s">
         <v>720</v>
       </c>
@@ -58799,7 +59078,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="614" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="614" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A614" t="s">
         <v>2258</v>
       </c>
@@ -58828,7 +59107,7 @@
         <v>2262</v>
       </c>
     </row>
-    <row r="615" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="615" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A615" t="s">
         <v>3062</v>
       </c>
@@ -58857,7 +59136,7 @@
         <v>3066</v>
       </c>
     </row>
-    <row r="616" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="616" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A616" t="s">
         <v>2671</v>
       </c>
@@ -58886,7 +59165,7 @@
         <v>2675</v>
       </c>
     </row>
-    <row r="617" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="617" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A617" t="s">
         <v>2934</v>
       </c>
@@ -58915,7 +59194,7 @@
         <v>2938</v>
       </c>
     </row>
-    <row r="618" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="618" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A618" t="s">
         <v>2203</v>
       </c>
@@ -58944,7 +59223,7 @@
         <v>2207</v>
       </c>
     </row>
-    <row r="619" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="619" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A619" t="s">
         <v>811</v>
       </c>
@@ -58973,7 +59252,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="620" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="620" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A620" t="s">
         <v>2516</v>
       </c>
@@ -59002,7 +59281,7 @@
         <v>2519</v>
       </c>
     </row>
-    <row r="621" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="621" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A621" t="s">
         <v>2930</v>
       </c>
@@ -59031,7 +59310,7 @@
         <v>2933</v>
       </c>
     </row>
-    <row r="622" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="622" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A622" t="s">
         <v>3047</v>
       </c>
@@ -59060,7 +59339,7 @@
         <v>3050</v>
       </c>
     </row>
-    <row r="623" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="623" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A623" t="s">
         <v>998</v>
       </c>
@@ -59089,7 +59368,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="624" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="624" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A624" t="s">
         <v>1164</v>
       </c>

</xml_diff>